<commit_message>
amp & detector BOM, datasheets
</commit_message>
<xml_diff>
--- a/Analog-Signal-Components/PAX/PAM-2025/PAM-modules/amplifier-module/amplifier-module-v3/amp-module-v3-BOM.xlsx
+++ b/Analog-Signal-Components/PAX/PAM-2025/PAM-modules/amplifier-module/amplifier-module-v3/amp-module-v3-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmart\Desktop\Studium\5. Praxissemester\Seti\PAM\Files_for_GitHub\PAM-2025\PAM-modules\amplifier-module\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin\Documents\ATA\gerb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64752C1-27A7-4768-B36A-8A4B4A025F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2C8B6B-B18C-41BB-80B5-8AD54B527A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4000" yWindow="-20620" windowWidth="28800" windowHeight="15290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="86">
   <si>
     <t>Type</t>
   </si>
@@ -169,18 +169,6 @@
     <t>amplifier, 23 dB</t>
   </si>
   <si>
-    <t>SMA connector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">530-142-1701-201 </t>
-  </si>
-  <si>
-    <t>Johnson/Cinch Connectivity Solutions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">142-1701-201 </t>
-  </si>
-  <si>
     <t>feed trough C</t>
   </si>
   <si>
@@ -293,6 +281,39 @@
   </si>
   <si>
     <t>ATC Technologies</t>
+  </si>
+  <si>
+    <t>Ferrite Bead, 600 Ω</t>
+  </si>
+  <si>
+    <t>HZ0805E601R-10</t>
+  </si>
+  <si>
+    <t>Laird-Signal Integrity Products</t>
+  </si>
+  <si>
+    <t>Female SMA connector</t>
+  </si>
+  <si>
+    <t>Male SMA connector</t>
+  </si>
+  <si>
+    <t>AT37PET-40E0103F04</t>
+  </si>
+  <si>
+    <t>Aaren Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT37PET-41E0103F04 </t>
+  </si>
+  <si>
+    <t>AT37PET-41E0103F04</t>
+  </si>
+  <si>
+    <t>APC Technology</t>
+  </si>
+  <si>
+    <t>(GBP)</t>
   </si>
 </sst>
 </file>
@@ -417,8 +438,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -696,37 +717,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="20.59765625" customWidth="1"/>
-    <col min="3" max="3" width="22.265625" customWidth="1"/>
-    <col min="4" max="4" width="16.53125" customWidth="1"/>
-    <col min="5" max="5" width="31.46484375" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.1328125" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.06640625" customWidth="1"/>
-    <col min="10" max="10" width="9.06640625" customWidth="1"/>
-    <col min="11" max="11" width="9.46484375" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -758,9 +779,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -790,9 +811,9 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -822,9 +843,9 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -855,9 +876,9 @@
       </c>
       <c r="L6" s="7"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
@@ -887,9 +908,9 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -919,9 +940,9 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>36</v>
@@ -951,366 +972,426 @@
         <v>235.8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="D10" s="11"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="D11" s="9"/>
-      <c r="F11" s="6"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="11">
+        <v>2012</v>
+      </c>
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D11" s="11"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11">
-        <f>+A4*J4+A5*J5+A6*J6+A7*J7+A8*J8+A9*J9</f>
-        <v>260.71000000000004</v>
-      </c>
-      <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D12" s="9"/>
       <c r="F12" s="6"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="I12" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12">
+        <f>+A4*J4+A5*J5+A6*J6+A7*J7+A8*J8+A9*J9</f>
+        <v>513.87</v>
+      </c>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F13" s="6"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I14" t="s">
-        <v>5</v>
-      </c>
-      <c r="J14">
-        <v>9.49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F14" s="6"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>42</v>
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>4</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
       <c r="I15" t="s">
-        <v>57</v>
-      </c>
-      <c r="J15">
-        <v>13.49</v>
-      </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>84</v>
+      </c>
+      <c r="J16">
+        <v>10.82</v>
+      </c>
+      <c r="K16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17">
+        <v>13.49</v>
+      </c>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="G18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>(A16+A15)*2</f>
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" t="s">
-        <v>5</v>
-      </c>
-      <c r="J16">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A17">
-        <f>A14*2</f>
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" s="4"/>
-      <c r="I17" t="s">
-        <v>60</v>
-      </c>
-      <c r="J17">
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19">
         <f>17.5/50</f>
         <v>0.35</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A18">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="14">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="14">
         <v>21202</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I18" t="s">
+      <c r="G20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" t="s">
         <v>5</v>
       </c>
-      <c r="J18">
+      <c r="J20">
         <v>5.08</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" t="s">
+    <row r="21" spans="1:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
         <v>60</v>
       </c>
-      <c r="F19" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J19">
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21">
         <f>8.86/100</f>
         <v>8.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A20">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" t="s">
+        <v>49</v>
+      </c>
+      <c r="I22" t="s">
         <v>70</v>
       </c>
-      <c r="C20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" t="s">
-        <v>72</v>
-      </c>
-      <c r="E20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" t="s">
-        <v>71</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" t="s">
-        <v>53</v>
-      </c>
-      <c r="I20" t="s">
-        <v>74</v>
-      </c>
-      <c r="J20">
+      <c r="J22">
         <f>153.46/180</f>
         <v>0.85255555555555562</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" t="s">
-        <v>53</v>
-      </c>
-      <c r="I22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="F23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" t="s">
-        <v>53</v>
-      </c>
-      <c r="I23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I24" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" t="s">
+        <v>49</v>
+      </c>
+      <c r="I25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>49</v>
+      </c>
+      <c r="I26" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1328,22 +1409,24 @@
     <hyperlink ref="H7" r:id="rId10" xr:uid="{634D1DF7-4E2E-460D-A7F6-ADA55E72548C}"/>
     <hyperlink ref="H8" r:id="rId11" xr:uid="{89CE1159-3C53-4A3D-9658-E19EDE9EE3C4}"/>
     <hyperlink ref="G8" r:id="rId12" xr:uid="{AF78A9D3-3691-43EB-9353-EA6FE2B65652}"/>
-    <hyperlink ref="G14" r:id="rId13" xr:uid="{D6D24302-405A-4664-9D0B-81B2A864EC57}"/>
-    <hyperlink ref="H14" r:id="rId14" xr:uid="{E2582FA7-CB87-4243-9C78-905CE71E4965}"/>
-    <hyperlink ref="G16" r:id="rId15" xr:uid="{2344F6E7-7CCD-4195-A038-E46C0AAD3CB5}"/>
-    <hyperlink ref="H16" r:id="rId16" xr:uid="{E4CF8212-66ED-4443-BC29-018D1AB7174A}"/>
-    <hyperlink ref="G15" r:id="rId17" xr:uid="{9CDC9DC5-066F-4C46-96F0-3081D293A4B1}"/>
-    <hyperlink ref="H15" r:id="rId18" xr:uid="{53C47AA7-FD41-491A-9EF9-270DD29D0386}"/>
-    <hyperlink ref="G18" r:id="rId19" xr:uid="{864F061D-4C2D-4E01-A419-510B15DA50A2}"/>
-    <hyperlink ref="H18" r:id="rId20" xr:uid="{BAC90AA8-AE47-4C24-B480-655972105C7F}"/>
-    <hyperlink ref="G19" r:id="rId21" xr:uid="{791D2FF6-8CA1-42D6-9144-75BEA3594CE8}"/>
-    <hyperlink ref="G17" r:id="rId22" xr:uid="{8AEC8668-8534-46CD-9B4A-C9523C444C68}"/>
-    <hyperlink ref="G22" r:id="rId23" xr:uid="{9E66B4E6-AB8E-4D98-A532-592A10558EC9}"/>
-    <hyperlink ref="G23" r:id="rId24" xr:uid="{E19A4C4A-DB86-4DC9-943E-42DD15B64480}"/>
-    <hyperlink ref="G24" r:id="rId25" xr:uid="{CE57D22D-4646-41E3-8925-B30E53CE92EF}"/>
-    <hyperlink ref="G20" r:id="rId26" xr:uid="{C8DFF2BB-6809-4F61-85A7-922F3AC18C80}"/>
+    <hyperlink ref="G18" r:id="rId13" xr:uid="{2344F6E7-7CCD-4195-A038-E46C0AAD3CB5}"/>
+    <hyperlink ref="H18" r:id="rId14" xr:uid="{E4CF8212-66ED-4443-BC29-018D1AB7174A}"/>
+    <hyperlink ref="G17" r:id="rId15" xr:uid="{9CDC9DC5-066F-4C46-96F0-3081D293A4B1}"/>
+    <hyperlink ref="H17" r:id="rId16" xr:uid="{53C47AA7-FD41-491A-9EF9-270DD29D0386}"/>
+    <hyperlink ref="G20" r:id="rId17" xr:uid="{864F061D-4C2D-4E01-A419-510B15DA50A2}"/>
+    <hyperlink ref="H20" r:id="rId18" xr:uid="{BAC90AA8-AE47-4C24-B480-655972105C7F}"/>
+    <hyperlink ref="G21" r:id="rId19" xr:uid="{791D2FF6-8CA1-42D6-9144-75BEA3594CE8}"/>
+    <hyperlink ref="G19" r:id="rId20" xr:uid="{8AEC8668-8534-46CD-9B4A-C9523C444C68}"/>
+    <hyperlink ref="G24" r:id="rId21" xr:uid="{9E66B4E6-AB8E-4D98-A532-592A10558EC9}"/>
+    <hyperlink ref="G25" r:id="rId22" xr:uid="{E19A4C4A-DB86-4DC9-943E-42DD15B64480}"/>
+    <hyperlink ref="G26" r:id="rId23" xr:uid="{CE57D22D-4646-41E3-8925-B30E53CE92EF}"/>
+    <hyperlink ref="G22" r:id="rId24" xr:uid="{C8DFF2BB-6809-4F61-85A7-922F3AC18C80}"/>
+    <hyperlink ref="G10" r:id="rId25" xr:uid="{F12F83FA-D5B5-47CB-95B6-33D0B0B99B49}"/>
+    <hyperlink ref="H10" r:id="rId26" xr:uid="{EEA2F635-A785-41D0-91D7-F6B9619E819F}"/>
+    <hyperlink ref="G16" r:id="rId27" xr:uid="{D6D24302-405A-4664-9D0B-81B2A864EC57}"/>
+    <hyperlink ref="H16" r:id="rId28" xr:uid="{7CA77FB8-DA43-4D12-9FE1-678C4D14EA52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId27"/>
+  <pageSetup orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>